<commit_message>
added estimators for time estimates and numerous other additions with mebrunet
</commit_message>
<xml_diff>
--- a/templates/excel-template.xlsx
+++ b/templates/excel-template.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$41</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>Building</t>
   </si>
@@ -180,6 +180,24 @@
   </si>
   <si>
     <t>Results Chart</t>
+  </si>
+  <si>
+    <t>Day Start</t>
+  </si>
+  <si>
+    <t>Night Start</t>
+  </si>
+  <si>
+    <t>Lab Occupancy Start</t>
+  </si>
+  <si>
+    <t>Lab Occupancy End</t>
+  </si>
+  <si>
+    <t>Hood Occupied (%)</t>
+  </si>
+  <si>
+    <t>Estimated Usage Parameters</t>
   </si>
 </sst>
 </file>
@@ -892,6 +910,75 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="305" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -901,58 +988,31 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -964,53 +1024,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="305" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="306">
@@ -1435,11 +1453,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="232620976"/>
-        <c:axId val="232617712"/>
+        <c:axId val="492315888"/>
+        <c:axId val="492327312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="232620976"/>
+        <c:axId val="492315888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1466,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232617712"/>
+        <c:crossAx val="492327312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1456,7 +1474,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="232617712"/>
+        <c:axId val="492327312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232620976"/>
+        <c:crossAx val="492315888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1490,15 +1508,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>6454</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
+      <xdr:colOff>828676</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>148644</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1521,8 +1539,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76200" y="28575"/>
-          <a:ext cx="1590675" cy="520119"/>
+          <a:off x="6454" y="0"/>
+          <a:ext cx="1660422" cy="542925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1886,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:F8"/>
+      <selection activeCell="E9" sqref="E9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1897,25 +1915,25 @@
     <col min="1" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32"/>
       <c r="B1" s="33"/>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="81"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
       <c r="F2" s="35" t="s">
         <v>31</v>
       </c>
@@ -1923,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -1932,96 +1950,156 @@
       <c r="F3" s="37"/>
       <c r="G3" s="38"/>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
+    <row r="4" spans="1:15" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="76"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="86"/>
+      <c r="I5" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="88"/>
+      <c r="K5" s="89"/>
+      <c r="M5" s="87" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="88"/>
+      <c r="O5" s="89"/>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="64" t="s">
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="88"/>
+      <c r="G6" s="89"/>
+      <c r="I6" s="100" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="101"/>
+      <c r="K6" s="71">
+        <v>10000</v>
+      </c>
+      <c r="M6" s="100"/>
+      <c r="N6" s="101"/>
+      <c r="O6" s="71"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="86" t="s">
+      <c r="C7" s="92"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="87"/>
-      <c r="G7" s="101">
+      <c r="F7" s="101"/>
+      <c r="G7" s="71">
         <v>10000</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="75"/>
+      <c r="K7" s="69">
+        <v>8.75</v>
+      </c>
+      <c r="M7" s="74"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="69"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="81">
+      <c r="B8" s="94">
         <v>200</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="88" t="s">
+      <c r="C8" s="95"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="89"/>
-      <c r="G8" s="99">
+      <c r="F8" s="75"/>
+      <c r="G8" s="69">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="77"/>
+      <c r="K8" s="72">
+        <v>10</v>
+      </c>
+      <c r="M8" s="76"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="72"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="90" t="s">
+      <c r="C9" s="98"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="91"/>
-      <c r="G9" s="102">
+      <c r="F9" s="77"/>
+      <c r="G9" s="72">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="74" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="75"/>
+      <c r="K9" s="73">
+        <v>4</v>
+      </c>
+      <c r="M9" s="74"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="73"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="88" t="s">
+      <c r="E10" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="89"/>
-      <c r="G10" s="103">
+      <c r="F10" s="75"/>
+      <c r="G10" s="73">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="77"/>
+      <c r="K10" s="70">
+        <v>200</v>
+      </c>
+      <c r="M10" s="76"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="70"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>47</v>
       </c>
@@ -2032,15 +2110,29 @@
       <c r="D11" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="90" t="s">
+      <c r="E11" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="91"/>
-      <c r="G11" s="100">
+      <c r="F11" s="77"/>
+      <c r="G11" s="70">
         <v>200</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="75"/>
+      <c r="K11" s="73">
+        <v>10</v>
+      </c>
+      <c r="M11" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="N11" s="75"/>
+      <c r="O11" s="73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
         <v>13</v>
       </c>
@@ -2051,15 +2143,29 @@
       <c r="D12" s="18">
         <v>72</v>
       </c>
-      <c r="E12" s="88" t="s">
+      <c r="E12" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="89"/>
-      <c r="G12" s="103">
+      <c r="F12" s="75"/>
+      <c r="G12" s="73">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="77"/>
+      <c r="K12" s="72">
+        <v>2</v>
+      </c>
+      <c r="M12" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="77"/>
+      <c r="O12" s="72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -2070,15 +2176,29 @@
       <c r="D13" s="19">
         <v>24</v>
       </c>
-      <c r="E13" s="90" t="s">
+      <c r="E13" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="91"/>
-      <c r="G13" s="102">
+      <c r="F13" s="77"/>
+      <c r="G13" s="72">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="75"/>
+      <c r="K13" s="64">
+        <v>5.25</v>
+      </c>
+      <c r="M13" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" s="75"/>
+      <c r="O13" s="64">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>15</v>
       </c>
@@ -2089,15 +2209,29 @@
       <c r="D14" s="20">
         <v>28</v>
       </c>
-      <c r="E14" s="88" t="s">
+      <c r="E14" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="89"/>
-      <c r="G14" s="94">
+      <c r="F14" s="75"/>
+      <c r="G14" s="64">
         <v>5.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="77"/>
+      <c r="K14" s="65">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M14" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="77"/>
+      <c r="O14" s="65">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
@@ -2108,15 +2242,29 @@
       <c r="D15" s="19">
         <v>1200</v>
       </c>
-      <c r="E15" s="90" t="s">
+      <c r="E15" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="91"/>
-      <c r="G15" s="95">
+      <c r="F15" s="77"/>
+      <c r="G15" s="65">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="75"/>
+      <c r="K15" s="66">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="M15" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="N15" s="75"/>
+      <c r="O15" s="66">
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
@@ -2127,15 +2275,25 @@
       <c r="D16" s="20">
         <v>300</v>
       </c>
-      <c r="E16" s="88" t="s">
+      <c r="E16" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="89"/>
-      <c r="G16" s="96">
+      <c r="F16" s="75"/>
+      <c r="G16" s="66">
         <v>0.91666666666666663</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="76"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="67"/>
+      <c r="M16" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="N16" s="77"/>
+      <c r="O16" s="67">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -2146,15 +2304,25 @@
       <c r="D17" s="19">
         <v>100</v>
       </c>
-      <c r="E17" s="90" t="s">
+      <c r="E17" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="91"/>
-      <c r="G17" s="97">
+      <c r="F17" s="77"/>
+      <c r="G17" s="67">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="78"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="68"/>
+      <c r="M17" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="79"/>
+      <c r="O17" s="68">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
         <v>20</v>
       </c>
@@ -2165,15 +2333,15 @@
       <c r="D18" s="21">
         <v>60</v>
       </c>
-      <c r="E18" s="92" t="s">
+      <c r="E18" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="93"/>
-      <c r="G18" s="98">
+      <c r="F18" s="79"/>
+      <c r="G18" s="68">
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
       <c r="B19" s="40"/>
       <c r="C19" s="45"/>
@@ -2182,38 +2350,38 @@
       <c r="F19" s="40"/>
       <c r="G19" s="40"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="69" t="s">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="71"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="64" t="s">
+      <c r="B20" s="84"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="90"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="65"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="64" t="s">
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="66"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="89"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="68"/>
+      <c r="C22" s="103"/>
       <c r="D22" s="54" t="s">
         <v>39</v>
       </c>
@@ -2227,7 +2395,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>1</v>
       </c>
@@ -2246,11 +2414,11 @@
         <v>10000</v>
       </c>
       <c r="G23" s="28">
-        <f t="shared" ref="G23:G29" si="0">$F$23-F23</f>
+        <f>$F$23-F23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>2</v>
       </c>
@@ -2265,15 +2433,15 @@
         <v>1000</v>
       </c>
       <c r="F24" s="23">
-        <f t="shared" ref="F24:F29" si="1">SUM(D24:E24)</f>
+        <f t="shared" ref="F24:F29" si="0">SUM(D24:E24)</f>
         <v>9000</v>
       </c>
       <c r="G24" s="29">
-        <f t="shared" si="0"/>
+        <f>$F$23-F24</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>3</v>
       </c>
@@ -2288,15 +2456,15 @@
         <v>0</v>
       </c>
       <c r="F25" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8000</v>
       </c>
       <c r="G25" s="30">
-        <f t="shared" si="0"/>
+        <f>$F$23-F25</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>4</v>
       </c>
@@ -2311,15 +2479,15 @@
         <v>2000</v>
       </c>
       <c r="F26" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8000</v>
       </c>
       <c r="G26" s="29">
-        <f t="shared" si="0"/>
+        <f>$F$23-F26</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>5</v>
       </c>
@@ -2334,15 +2502,15 @@
         <v>1000</v>
       </c>
       <c r="F27" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9000</v>
       </c>
       <c r="G27" s="30">
-        <f t="shared" si="0"/>
+        <f>$F$23-F27</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>6</v>
       </c>
@@ -2357,15 +2525,15 @@
         <v>500</v>
       </c>
       <c r="F28" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6500</v>
       </c>
       <c r="G28" s="29">
-        <f t="shared" si="0"/>
+        <f>$F$23-F28</f>
         <v>3500</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>7</v>
       </c>
@@ -2380,34 +2548,34 @@
         <v>0</v>
       </c>
       <c r="F29" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6000</v>
       </c>
       <c r="G29" s="31">
-        <f t="shared" si="0"/>
+        <f>$F$23-F29</f>
         <v>4000</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="69" t="s">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="70"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="69" t="s">
+      <c r="B31" s="84"/>
+      <c r="C31" s="90"/>
+      <c r="D31" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="71"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="84"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="90"/>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="34"/>
       <c r="B32" s="2"/>
       <c r="C32" s="39"/>
@@ -2593,12 +2761,39 @@
     <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
+  <mergeCells count="52">
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:G31"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A5:G5"/>
@@ -2615,11 +2810,10 @@
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>